<commit_message>
Mini rev. C1: change IC3 on the BOM
</commit_message>
<xml_diff>
--- a/belamini/belamini_cape_rev_C1/belamini_cape_C1_bom.xlsx
+++ b/belamini/belamini_cape_rev_C1/belamini_cape_C1_bom.xlsx
@@ -190,25 +190,25 @@
     <t>IC3</t>
   </si>
   <si>
-    <t>AD7699</t>
-  </si>
-  <si>
-    <t>LFCSP-20</t>
+    <t>ADS8168IRHBT</t>
+  </si>
+  <si>
+    <t>QFN-32</t>
   </si>
   <si>
     <t>16-bit ADC</t>
   </si>
   <si>
-    <t>584-AD7699BCPZ</t>
+    <t>595-ADS8168IRHBT</t>
+  </si>
+  <si>
+    <t>Other parts in ADS816x series may also work.</t>
   </si>
   <si>
     <t>IC4</t>
   </si>
   <si>
     <t>TLV320AIC3104</t>
-  </si>
-  <si>
-    <t>QFN-32</t>
   </si>
   <si>
     <t>Audio codec</t>
@@ -2084,7 +2084,9 @@
       <c r="H14" t="s" s="6">
         <v>62</v>
       </c>
-      <c r="I14" s="5"/>
+      <c r="I14" t="s" s="6">
+        <v>63</v>
+      </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
@@ -2093,19 +2095,19 @@
     </row>
     <row r="15" ht="15" customHeight="1">
       <c r="A15" t="s" s="7">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B15" s="8">
         <v>1</v>
       </c>
       <c r="C15" t="s" s="6">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s" s="6">
         <v>12</v>
       </c>
       <c r="E15" t="s" s="6">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F15" t="s" s="6">
         <v>66</v>

</xml_diff>